<commit_message>
adjusted due to changes on scraped website
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,10 +641,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>30598523</t>
-        </is>
+      <c r="A2" t="n">
+        <v>30598523</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -656,20 +654,16 @@
           <t>პ.სააკაძის ქ.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="D2" t="n">
+        <v>29</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>500 $</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="F2" t="n">
+        <v>250</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -686,161 +680,351 @@
           <t>ბინა მდებარეობს კავკასიის უნივერსიტეტთან. ახალი რემონტი, ყველა საჭირო ავეჯი და ტექნიკა არის ბინაში.</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>60 მ²</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>7</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>ახალი რემონტით</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>ახალი აშენებული</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>უძრავი ქონება</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>ბინა</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>ქირავდება</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>https://home.ss.ge/ka/udzravi-qoneba/30603775</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>31024583</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ქირავდება 2 ოთახიანი ბინა ისანში</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ბერი გაბრიელ სალოსის გამზ.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1,200 ₾</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>558 46 27 74</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nini</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ს ა ს წ რ ა ფ ო დ !!! ისანში ბერი გაბრიელ სალოსის გამზირზე ქირავდება 2 ოთახიანი ბინა 1 საძინებელი ოთახით,ავეჯით,ტექნიკით,ცენტრალური გათბობის სიტემით,კეთილმოწყობილი შლაგბაუმიანი ეზოთი,კოდირებული კარით,ვიდეომონიტორინგით სადარბაზოში,მიმდებარედ ყველანაირი ობიექტით.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>sdadasd</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>56 მ²</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>ახალი რემონტით</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>ახალი აშენებული</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>უძრავი ქონება</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>ბინა</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>ქირავდება</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>კი</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>https://home.ss.ge/ka/udzravi-qoneba/30603775</t>
-        </is>
-      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>არა</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>არა</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>არა</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>არა</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>არა</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>კი</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>